<commit_message>
Added tests for timestamps and Picarro resampling
</commit_message>
<xml_diff>
--- a/data/agage_test/data_release_schedule.xlsx
+++ b/data/agage_test/data_release_schedule.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E35A2-C7C4-6D4B-92C7-5E3F94A04A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F333A7CE-DCC8-E049-A5FE-413ABE74A5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="2240" windowWidth="27240" windowHeight="16440" activeTab="3" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="820" yWindow="2240" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="6" r:id="rId1"/>
     <sheet name="GAGE" sheetId="7" r:id="rId2"/>
     <sheet name="GCMD" sheetId="8" r:id="rId3"/>
     <sheet name="GCMS-Medusa" sheetId="4" r:id="rId4"/>
+    <sheet name="Picarro" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>MHD</t>
   </si>
@@ -1053,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEEAF2A-BA72-FC4F-92D8-D72395398919}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,4 +1134,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E10A2C-139C-F044-B81B-60293FE9932E}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes in inlet grouping function, and test added
</commit_message>
<xml_diff>
--- a/data/agage_test/data_release_schedule.xlsx
+++ b/data/agage_test/data_release_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/dagage2_home/code/agage-archive/data/agage_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F333A7CE-DCC8-E049-A5FE-413ABE74A5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51126B84-9984-E642-802F-667BD15DEB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="2240" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
   <si>
     <t>MHD</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>h2</t>
+  </si>
+  <si>
+    <t>TAC</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E10A2C-139C-F044-B81B-60293FE9932E}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,37 +1153,37 @@
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1188,15 +1191,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>

</xml_diff>